<commit_message>
updated / added daily Odean calculation
</commit_message>
<xml_diff>
--- a/reports/df_tstat_results_daily_2020-07-26_16_47_07.xlsx
+++ b/reports/df_tstat_results_daily_2020-07-26_16_47_07.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://fhjoanneum-my.sharepoint.com/personal/juergen_schatzmann_edu_fh-joanneum_at/Documents/02 Statistik/CryptoDispGitHub/CryptoDisposition/reports/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jes/OneDrive - FH JOANNEUM/02 Statistik/CryptoDispGitHub/CryptoDisposition/reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="11_588FD194480C8901B3FA9D5CAF9D4DDC3048E2DD" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8BC9692F-C738-3144-8CE7-D74D3615AC45}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D68C70D1-6270-2048-90F5-38C6046373C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25520" windowHeight="27280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25600" yWindow="460" windowWidth="25520" windowHeight="27280" firstSheet="44" activeTab="49" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="00_Summary" sheetId="1" r:id="rId1"/>
@@ -1221,7 +1221,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -33179,7 +33179,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3100-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -37719,7 +37719,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:G85"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>